<commit_message>
ENH: Add dynamic lapse
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/input_tables/assumptions_202312.xlsx
+++ b/lifelib/libraries/appliedlife/input_tables/assumptions_202312.xlsx
@@ -1,24 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e058ec69bd94c7d/pyproj/lifelib/lifelib/libraries/appliedlife/input_tables/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\input_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{E5F043AF-D92A-411B-B2F7-38180FF25FC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{65039F03-801B-4FDE-8B0A-7BE7F683EAEA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBEFF7CA-1C24-415E-8401-85E25E1A28EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6411" yWindow="2134" windowWidth="26529" windowHeight="15652" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inflation" sheetId="1" r:id="rId1"/>
     <sheet name="Mortality" sheetId="2" r:id="rId2"/>
     <sheet name="Lapse" sheetId="4" r:id="rId3"/>
-    <sheet name="ADB" sheetId="3" r:id="rId4"/>
-    <sheet name="CI" sheetId="6" r:id="rId5"/>
-    <sheet name="Expense" sheetId="5" r:id="rId6"/>
+    <sheet name="DynLapse" sheetId="7" r:id="rId4"/>
+    <sheet name="ADB" sheetId="3" r:id="rId5"/>
+    <sheet name="CI" sheetId="6" r:id="rId6"/>
+    <sheet name="Expense" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="28">
   <si>
     <t>DE</t>
   </si>
@@ -80,6 +81,51 @@
   </si>
   <si>
     <t>M004</t>
+  </si>
+  <si>
+    <t>DL001A</t>
+  </si>
+  <si>
+    <t>DL001B</t>
+  </si>
+  <si>
+    <t>DL002A</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>FactorCap</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>FactorFloor</t>
+  </si>
+  <si>
+    <t>DL002B</t>
+  </si>
+  <si>
+    <t>formula_id</t>
+  </si>
+  <si>
+    <t>DL001</t>
+  </si>
+  <si>
+    <t>DL002</t>
   </si>
 </sst>
 </file>
@@ -406,7 +452,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E151"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -3273,7 +3319,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ACC3179-CEEC-4987-8B9E-F4BD51E47B9D}">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
@@ -3572,6 +3618,134 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C978DAB-7A7E-4CE2-896C-CC4A072949B8}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="1" max="2" width="12.84375" customWidth="1"/>
+    <col min="8" max="8" width="10.23046875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="B1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E2">
+        <v>3.5</v>
+      </c>
+      <c r="F2">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E3">
+        <v>0.7</v>
+      </c>
+      <c r="F3">
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="G4">
+        <v>1.5</v>
+      </c>
+      <c r="H4">
+        <v>0.8</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>0.5</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8CE630C-EEA1-4AF5-B714-0D3DC3945FCA}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3583,7 +3757,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0759C15-CDDB-4203-9894-69E8546D59F2}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -3595,7 +3769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0E1E27E-D71D-44A9-B1AE-3025E478762A}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>